<commit_message>
ARI analysis with 1000 instead of 100 runs
</commit_message>
<xml_diff>
--- a/ARIevaluation/PrioTopK/output/topkanalysis.xlsx
+++ b/ARIevaluation/PrioTopK/output/topkanalysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\javaworkspace\PrioTopK\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\TraceSec\tracesec-prioritization\ARIevaluation\PrioTopK\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7081E30-F3A6-4CC7-B48C-9B78468E2FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECDD151-2BA7-48A5-BCB3-0020E9232616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{9F6FB41D-B757-4B1F-BB02-0258B271A8C4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{9F6FB41D-B757-4B1F-BB02-0258B271A8C4}"/>
   </bookViews>
   <sheets>
     <sheet name="itrust" sheetId="3" r:id="rId1"/>
@@ -106,10 +106,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1674,6 +1674,7 @@
         <c:axId val="528934320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.45"/>
           <c:min val="-0.1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3413,7 +3414,7 @@
         <c:axId val="528943440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.5"/>
+          <c:max val="0.45"/>
           <c:min val="-0.1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -31091,8 +31092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39CD883-F74C-47E5-932D-444A56709C19}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31102,14 +31103,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -31118,13 +31119,13 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -31133,19 +31134,19 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$B$2:$B$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$B$2:$B$1001)</f>
         <v>0.14547253834735224</v>
       </c>
       <c r="C3">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$B$2:$B$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$B$2:$B$1001)</f>
         <v>7.3674395964506381E-2</v>
       </c>
       <c r="D3">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$B$2:$B$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$B$2:$B$1001)</f>
         <v>-1.4411182582880201E-2</v>
       </c>
       <c r="E3">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$B$2:$B$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$B$2:$B$1001)</f>
         <v>6.9293960224273865E-2</v>
       </c>
     </row>
@@ -31154,19 +31155,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$A$2:$A$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$A$2:$A$1001)</f>
         <v>0.14932097594232027</v>
       </c>
       <c r="C4">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$A$2:$A$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$A$2:$A$1001)</f>
         <v>8.3777125409855005E-2</v>
       </c>
       <c r="D4">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$A$2:$A$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$A$2:$A$1001)</f>
         <v>-1.6561562382419442E-3</v>
       </c>
       <c r="E4">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$A$2:$A$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$A$2:$A$1001)</f>
         <v>7.5900099257370651E-2</v>
       </c>
     </row>
@@ -31175,19 +31176,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$C$2:$C$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$C$2:$C$1001)</f>
         <v>0.15454460569465642</v>
       </c>
       <c r="C5">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$C$2:$C$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$C$2:$C$1001)</f>
         <v>9.8975420584322224E-2</v>
       </c>
       <c r="D5">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$C$2:$C$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$C$2:$C$1001)</f>
         <v>6.8420203780781119E-2</v>
       </c>
       <c r="E5">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$C$2:$C$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$C$2:$C$1001)</f>
         <v>9.2878585564539262E-2</v>
       </c>
     </row>
@@ -31196,19 +31197,19 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$D$2:$D$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$D$2:$D$1001)</f>
         <v>0.19704510339909614</v>
       </c>
       <c r="C6">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$D$2:$D$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$D$2:$D$1001)</f>
         <v>8.9972616848872256E-2</v>
       </c>
       <c r="D6">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$D$2:$D$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$D$2:$D$1001)</f>
         <v>0.13782646482053665</v>
       </c>
       <c r="E6">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$D$2:$D$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$D$2:$D$1001)</f>
         <v>8.560327922685379E-2</v>
       </c>
     </row>
@@ -31217,19 +31218,19 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$E$2:$E$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$E$2:$E$1001)</f>
         <v>0.26811244211980328</v>
       </c>
       <c r="C7">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$E$2:$E$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$E$2:$E$1001)</f>
         <v>7.7663859249626072E-2</v>
       </c>
       <c r="D7">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$E$2:$E$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$E$2:$E$1001)</f>
         <v>0.2127353739691179</v>
       </c>
       <c r="E7">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$E$2:$E$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$E$2:$E$1001)</f>
         <v>6.5701749244413313E-2</v>
       </c>
     </row>
@@ -31238,19 +31239,19 @@
         <v>25</v>
       </c>
       <c r="B8">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$F$2:$F$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$F$2:$F$1001)</f>
         <v>0.35668970103867587</v>
       </c>
       <c r="C8">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$F$2:$F$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$F$2:$F$1001)</f>
         <v>4.8509270337876942E-2</v>
       </c>
       <c r="D8">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$F$2:$F$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$F$2:$F$1001)</f>
         <v>0.30411210946571132</v>
       </c>
       <c r="E8">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$F$2:$F$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$F$2:$F$1001)</f>
         <v>4.6000658900812924E-2</v>
       </c>
     </row>
@@ -31259,19 +31260,19 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$G$2:$G$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$G$2:$G$1001)</f>
         <v>0.34139722578549608</v>
       </c>
       <c r="C9">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$G$2:$G$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$G$2:$G$1001)</f>
         <v>1.1102230246251565E-16</v>
       </c>
       <c r="D9">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$G$2:$G$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$G$2:$G$1001)</f>
         <v>0.30578328076984657</v>
       </c>
       <c r="E9">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$G$2:$G$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$G$2:$G$1001)</f>
         <v>4.4497534575950848E-2</v>
       </c>
     </row>
@@ -31280,19 +31281,19 @@
         <v>35</v>
       </c>
       <c r="B10">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$H$2:$H$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$H$2:$H$1001)</f>
         <v>0.23602991543839669</v>
       </c>
       <c r="C10">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$H$2:$H$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$H$2:$H$1001)</f>
         <v>2.9635753171232997E-2</v>
       </c>
       <c r="D10">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$H$2:$H$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$H$2:$H$1001)</f>
         <v>0.19286629582388451</v>
       </c>
       <c r="E10">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$H$2:$H$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$H$2:$H$1001)</f>
         <v>5.01231640414617E-2</v>
       </c>
     </row>
@@ -31301,19 +31302,19 @@
         <v>40</v>
       </c>
       <c r="B11">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$I$2:$I$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$I$2:$I$1001)</f>
         <v>0.2032607980185831</v>
       </c>
       <c r="C11">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$I$2:$I$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$I$2:$I$1001)</f>
         <v>1.8591659000537889E-2</v>
       </c>
       <c r="D11">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$I$2:$I$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$I$2:$I$1001)</f>
         <v>9.5536962173390305E-2</v>
       </c>
       <c r="E11">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$I$2:$I$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$I$2:$I$1001)</f>
         <v>3.4886804588892303E-2</v>
       </c>
     </row>
@@ -31322,19 +31323,19 @@
         <v>45</v>
       </c>
       <c r="B12">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$J$2:$J$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$J$2:$J$1001)</f>
         <v>0.15562519834972971</v>
       </c>
       <c r="C12">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$J$2:$J$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$J$2:$J$1001)</f>
         <v>2.847636915277036E-2</v>
       </c>
       <c r="D12">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$J$2:$J$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$J$2:$J$1001)</f>
         <v>5.1171291888524456E-2</v>
       </c>
       <c r="E12">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$J$2:$J$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$J$2:$J$1001)</f>
         <v>3.032717313399871E-2</v>
       </c>
     </row>
@@ -31343,19 +31344,19 @@
         <v>50</v>
       </c>
       <c r="B13">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$K$2:$K$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$K$2:$K$1001)</f>
         <v>0.10325305152660792</v>
       </c>
       <c r="C13">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$K$2:$K$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$K$2:$K$1001)</f>
         <v>3.6731020840490687E-2</v>
       </c>
       <c r="D13">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$K$2:$K$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$K$2:$K$1001)</f>
         <v>2.5459877953629473E-2</v>
       </c>
       <c r="E13">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$K$2:$K$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$K$2:$K$1001)</f>
         <v>2.7046891643746074E-2</v>
       </c>
     </row>
@@ -31364,19 +31365,19 @@
         <v>55</v>
       </c>
       <c r="B14">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$L$2:$L$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$L$2:$L$1001)</f>
         <v>5.9456168831168721E-2</v>
       </c>
       <c r="C14">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$L$2:$L$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$L$2:$L$1001)</f>
         <v>3.344027074132002E-2</v>
       </c>
       <c r="D14">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$L$2:$L$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$L$2:$L$1001)</f>
         <v>1.6093696126881895E-2</v>
       </c>
       <c r="E14">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$L$2:$L$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$L$2:$L$1001)</f>
         <v>2.1954762352262493E-2</v>
       </c>
     </row>
@@ -31385,19 +31386,19 @@
         <v>60</v>
       </c>
       <c r="B15">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$M$2:$M$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$M$2:$M$1001)</f>
         <v>6.7526386806376057E-2</v>
       </c>
       <c r="C15">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$M$2:$M$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$M$2:$M$1001)</f>
         <v>3.8450788039703865E-2</v>
       </c>
       <c r="D15">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$M$2:$M$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$M$2:$M$1001)</f>
         <v>8.641835429906734E-3</v>
       </c>
       <c r="E15">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$M$2:$M$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$M$2:$M$1001)</f>
         <v>1.9146679704781504E-2</v>
       </c>
     </row>
@@ -31406,19 +31407,19 @@
         <v>65</v>
       </c>
       <c r="B16">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$N$2:$N$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$N$2:$N$1001)</f>
         <v>6.1317986174514089E-2</v>
       </c>
       <c r="C16">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$N$2:$N$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$N$2:$N$1001)</f>
         <v>3.9632516614715209E-2</v>
       </c>
       <c r="D16">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$N$2:$N$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$N$2:$N$1001)</f>
         <v>1.31407330116082E-2</v>
       </c>
       <c r="E16">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$N$2:$N$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$N$2:$N$1001)</f>
         <v>2.3613275756784357E-2</v>
       </c>
     </row>
@@ -31427,19 +31428,19 @@
         <v>70</v>
       </c>
       <c r="B17">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$O$2:$O$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$O$2:$O$1001)</f>
         <v>7.2146664742567257E-2</v>
       </c>
       <c r="C17">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$O$2:$O$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$O$2:$O$1001)</f>
         <v>4.3001863515958159E-2</v>
       </c>
       <c r="D17">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$O$2:$O$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$O$2:$O$1001)</f>
         <v>1.3021772616159397E-2</v>
       </c>
       <c r="E17">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$O$2:$O$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$O$2:$O$1001)</f>
         <v>3.0506241159845057E-2</v>
       </c>
     </row>
@@ -31448,19 +31449,19 @@
         <v>75</v>
       </c>
       <c r="B18">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$P$2:$P$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$P$2:$P$1001)</f>
         <v>7.3673792807354102E-2</v>
       </c>
       <c r="C18">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$P$2:$P$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$P$2:$P$1001)</f>
         <v>4.8977742958372074E-2</v>
       </c>
       <c r="D18" s="1">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$P$2:$P$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$P$2:$P$1001)</f>
         <v>1.0785496009698059E-2</v>
       </c>
       <c r="E18">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$P$2:$P$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$P$2:$P$1001)</f>
         <v>3.4363434621418325E-2</v>
       </c>
     </row>
@@ -31469,19 +31470,19 @@
         <v>80</v>
       </c>
       <c r="B19">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$Q$2:$Q$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$Q$2:$Q$1001)</f>
         <v>9.8774004296385221E-2</v>
       </c>
       <c r="C19">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$Q$2:$Q$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$Q$2:$Q$1001)</f>
         <v>3.8901602817265429E-2</v>
       </c>
       <c r="D19">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$Q$2:$Q$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$Q$2:$Q$1001)</f>
         <v>1.1759340695136624E-2</v>
       </c>
       <c r="E19">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$Q$2:$Q$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$Q$2:$Q$1001)</f>
         <v>4.9735134601080144E-2</v>
       </c>
     </row>
@@ -31490,19 +31491,19 @@
         <v>85</v>
       </c>
       <c r="B20">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$R$2:$R$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$R$2:$R$1001)</f>
         <v>9.263945772500623E-2</v>
       </c>
       <c r="C20">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$R$2:$R$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$R$2:$R$1001)</f>
         <v>4.5326919415885396E-2</v>
       </c>
       <c r="D20">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$R$2:$R$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$R$2:$R$1001)</f>
         <v>1.4232900475900711E-2</v>
       </c>
       <c r="E20">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$R$2:$R$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$R$2:$R$1001)</f>
         <v>7.0147064208879853E-2</v>
       </c>
     </row>
@@ -31511,19 +31512,19 @@
         <v>90</v>
       </c>
       <c r="B21">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$S$2:$S$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$S$2:$S$1001)</f>
         <v>0.11165111818706581</v>
       </c>
       <c r="C21">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$S$2:$S$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$S$2:$S$1001)</f>
         <v>8.3436850647333E-2</v>
       </c>
       <c r="D21">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$S$2:$S$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$S$2:$S$1001)</f>
         <v>-2.0932589560040533E-2</v>
       </c>
       <c r="E21">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$S$2:$S$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$S$2:$S$1001)</f>
         <v>7.2889251620383677E-2</v>
       </c>
     </row>
@@ -31532,19 +31533,19 @@
         <v>95</v>
       </c>
       <c r="B22">
-        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$T$2:$T$101)</f>
+        <f>AVERAGE('[1]ari-eval-tracesec-itrust'!$T$2:$T$1001)</f>
         <v>9.0654771681996524E-2</v>
       </c>
       <c r="C22">
-        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$T$2:$T$101)</f>
+        <f>_xlfn.STDEV.P('[1]ari-eval-tracesec-itrust'!$T$2:$T$1001)</f>
         <v>0.15738520347472759</v>
       </c>
       <c r="D22">
-        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$T$2:$T$101)</f>
+        <f>AVERAGE('[2]ari-eval-sonarcube-itrust'!$T$2:$T$1001)</f>
         <v>-2.6789380749014984E-2</v>
       </c>
       <c r="E22">
-        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$T$2:$T$101)</f>
+        <f>_xlfn.STDEV.P('[2]ari-eval-sonarcube-itrust'!$T$2:$T$1001)</f>
         <v>5.2915551091664355E-2</v>
       </c>
     </row>
@@ -31566,8 +31567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9864635-2355-44AC-9B5A-8CDFEFA8D606}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31577,14 +31578,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -31593,13 +31594,13 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -31608,19 +31609,19 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$B$2:$B$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$B$2:$B$1001)</f>
         <v>8.5142348057643868E-2</v>
       </c>
       <c r="C3">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$B$2:$B$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$B$2:$B$1001)</f>
         <v>0.12867261615639375</v>
       </c>
       <c r="D3">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$B$2:$B$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$B$2:$B$1001)</f>
         <v>-5.6038533834586284E-2</v>
       </c>
       <c r="E3">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$B$2:$B$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$B$2:$B$1001)</f>
         <v>8.3266726846886741E-17</v>
       </c>
     </row>
@@ -31629,19 +31630,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$A$2:$A$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$A$2:$A$1001)</f>
         <v>0.12252122538353798</v>
       </c>
       <c r="C4">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$A$2:$A$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$A$2:$A$1001)</f>
         <v>0.11973861986098269</v>
       </c>
       <c r="D4">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$B$2:$B$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$B$2:$B$1001)</f>
         <v>-5.6038533834586284E-2</v>
       </c>
       <c r="E4">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$A$2:$A$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$A$2:$A$1001)</f>
         <v>4.2588895335479784E-2</v>
       </c>
     </row>
@@ -31650,19 +31651,19 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$C$2:$C$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$C$2:$C$1001)</f>
         <v>0.15589590486142138</v>
       </c>
       <c r="C5">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$C$2:$C$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$C$2:$C$1001)</f>
         <v>0.10086693732254118</v>
       </c>
       <c r="D5">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$C$2:$C$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$C$2:$C$1001)</f>
         <v>-1.6825894412103729E-3</v>
       </c>
       <c r="E5">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$C$2:$C$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$C$2:$C$1001)</f>
         <v>7.2468542601595951E-2</v>
       </c>
     </row>
@@ -31671,19 +31672,19 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$D$2:$D$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$D$2:$D$1001)</f>
         <v>0.23060557149689029</v>
       </c>
       <c r="C6">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$D$2:$D$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$D$2:$D$1001)</f>
         <v>5.9988658329439726E-2</v>
       </c>
       <c r="D6">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$D$2:$D$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$D$2:$D$1001)</f>
         <v>1.5741072851904736E-2</v>
       </c>
       <c r="E6">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$D$2:$D$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$D$2:$D$1001)</f>
         <v>6.7610192502172622E-2</v>
       </c>
     </row>
@@ -31692,19 +31693,19 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$E$2:$E$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$E$2:$E$1001)</f>
         <v>0.33369542178889267</v>
       </c>
       <c r="C7">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$E$2:$E$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$E$2:$E$1001)</f>
         <v>3.3306690738754696E-16</v>
       </c>
       <c r="D7">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$E$2:$E$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$E$2:$E$1001)</f>
         <v>3.8826656775469842E-2</v>
       </c>
       <c r="E7">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$E$2:$E$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$E$2:$E$1001)</f>
         <v>5.1144762478002467E-2</v>
       </c>
     </row>
@@ -31713,19 +31714,19 @@
         <v>25</v>
       </c>
       <c r="B8">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$F$2:$F$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$F$2:$F$1001)</f>
         <v>0.19840752688171931</v>
       </c>
       <c r="C8">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$F$2:$F$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$F$2:$F$1001)</f>
         <v>3.1189331631568264E-2</v>
       </c>
       <c r="D8">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$F$2:$F$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$F$2:$F$1001)</f>
         <v>5.5545574855252126E-2</v>
       </c>
       <c r="E8">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$F$2:$F$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$F$2:$F$1001)</f>
         <v>5.5682156262949339E-2</v>
       </c>
     </row>
@@ -31734,19 +31735,19 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$G$2:$G$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$G$2:$G$1001)</f>
         <v>0.19154425883256462</v>
       </c>
       <c r="C9">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$G$2:$G$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$G$2:$G$1001)</f>
         <v>3.9077050110947996E-2</v>
       </c>
       <c r="D9">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$G$2:$G$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$G$2:$G$1001)</f>
         <v>5.0127128136200579E-2</v>
       </c>
       <c r="E9">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$G$2:$G$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$G$2:$G$1001)</f>
         <v>4.4172942829946195E-2</v>
       </c>
     </row>
@@ -31755,19 +31756,19 @@
         <v>35</v>
       </c>
       <c r="B10">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$H$2:$H$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$H$2:$H$1001)</f>
         <v>0.17208636894061183</v>
       </c>
       <c r="C10">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$H$2:$H$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$H$2:$H$1001)</f>
         <v>1.6841959535943776E-2</v>
       </c>
       <c r="D10">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$H$2:$H$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$H$2:$H$1001)</f>
         <v>3.7176017914025229E-2</v>
       </c>
       <c r="E10">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$H$2:$H$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$H$2:$H$1001)</f>
         <v>2.9734826227852972E-2</v>
       </c>
     </row>
@@ -31776,19 +31777,19 @@
         <v>40</v>
       </c>
       <c r="B11">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$I$2:$I$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$I$2:$I$1001)</f>
         <v>0.14653937910035436</v>
       </c>
       <c r="C11">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$I$2:$I$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$I$2:$I$1001)</f>
         <v>3.0944394382645218E-2</v>
       </c>
       <c r="D11">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$I$2:$I$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$I$2:$I$1001)</f>
         <v>4.0370012870012843E-2</v>
       </c>
       <c r="E11">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$I$2:$I$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$I$2:$I$1001)</f>
         <v>3.1591995460654589E-2</v>
       </c>
     </row>
@@ -31797,19 +31798,19 @@
         <v>45</v>
       </c>
       <c r="B12">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$J$2:$J$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$J$2:$J$1001)</f>
         <v>0.10964403350272875</v>
       </c>
       <c r="C12">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$J$2:$J$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$J$2:$J$1001)</f>
         <v>3.4343734632924894E-2</v>
       </c>
       <c r="D12">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$J$2:$J$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$J$2:$J$1001)</f>
         <v>4.7909137963485657E-2</v>
       </c>
       <c r="E12">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$J$2:$J$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$J$2:$J$1001)</f>
         <v>3.1631863482203086E-2</v>
       </c>
     </row>
@@ -31818,19 +31819,19 @@
         <v>50</v>
       </c>
       <c r="B13">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$K$2:$K$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$K$2:$K$1001)</f>
         <v>8.4939999999999807E-2</v>
       </c>
       <c r="C13">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$K$2:$K$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$K$2:$K$1001)</f>
         <v>3.0928298587505169E-2</v>
       </c>
       <c r="D13">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$K$2:$K$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$K$2:$K$1001)</f>
         <v>7.3738901960784156E-2</v>
       </c>
       <c r="E13">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$K$2:$K$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$K$2:$K$1001)</f>
         <v>3.1706922282435046E-2</v>
       </c>
     </row>
@@ -31839,19 +31840,19 @@
         <v>55</v>
       </c>
       <c r="B14">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$L$2:$L$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$L$2:$L$1001)</f>
         <v>9.4095457682413966E-2</v>
       </c>
       <c r="C14">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$L$2:$L$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$L$2:$L$1001)</f>
         <v>1.9314631224775343E-2</v>
       </c>
       <c r="D14">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$L$2:$L$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$L$2:$L$1001)</f>
         <v>0.10039251207729435</v>
       </c>
       <c r="E14">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$L$2:$L$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$L$2:$L$1001)</f>
         <v>2.7848959709662158E-2</v>
       </c>
     </row>
@@ -31860,19 +31861,19 @@
         <v>60</v>
       </c>
       <c r="B15">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$M$2:$M$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$M$2:$M$1001)</f>
         <v>6.5340823440738646E-2</v>
       </c>
       <c r="C15">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$M$2:$M$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$M$2:$M$1001)</f>
         <v>2.0295602551673127E-2</v>
       </c>
       <c r="D15">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$M$2:$M$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$M$2:$M$1001)</f>
         <v>0.13774762891778106</v>
       </c>
       <c r="E15">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$M$2:$M$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$M$2:$M$1001)</f>
         <v>3.7305796781177521E-2</v>
       </c>
     </row>
@@ -31881,19 +31882,19 @@
         <v>65</v>
       </c>
       <c r="B16">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$N$2:$N$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$N$2:$N$1001)</f>
         <v>0.10494825733876816</v>
       </c>
       <c r="C16">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$N$2:$N$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$N$2:$N$1001)</f>
         <v>3.6170736318086663E-2</v>
       </c>
       <c r="D16">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$N$2:$N$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$N$2:$N$1001)</f>
         <v>0.16524283502385628</v>
       </c>
       <c r="E16">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$N$2:$N$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$N$2:$N$1001)</f>
         <v>4.7453942117821259E-2</v>
       </c>
     </row>
@@ -31902,19 +31903,19 @@
         <v>70</v>
       </c>
       <c r="B17">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$O$2:$O$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$O$2:$O$1001)</f>
         <v>9.8403353913434757E-2</v>
       </c>
       <c r="C17">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$O$2:$O$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$O$2:$O$1001)</f>
         <v>4.6328677795507166E-2</v>
       </c>
       <c r="D17">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$O$2:$O$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$O$2:$O$1001)</f>
         <v>0.1991419062319115</v>
       </c>
       <c r="E17">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$O$2:$O$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$O$2:$O$1001)</f>
         <v>6.3328218307908413E-2</v>
       </c>
     </row>
@@ -31923,19 +31924,19 @@
         <v>75</v>
       </c>
       <c r="B18">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$P$2:$P$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$P$2:$P$1001)</f>
         <v>8.811428571428552E-2</v>
       </c>
       <c r="C18">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$P$2:$P$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$P$2:$P$1001)</f>
         <v>5.2351133696630102E-2</v>
       </c>
       <c r="D18" s="1">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$P$2:$P$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$P$2:$P$1001)</f>
         <v>0.22296658312447701</v>
       </c>
       <c r="E18">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$P$2:$P$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$P$2:$P$1001)</f>
         <v>7.924567131691275E-2</v>
       </c>
     </row>
@@ -31944,19 +31945,19 @@
         <v>80</v>
       </c>
       <c r="B19">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$Q$2:$Q$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$Q$2:$Q$1001)</f>
         <v>7.4748317316344473E-2</v>
       </c>
       <c r="C19">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$Q$2:$Q$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$Q$2:$Q$1001)</f>
         <v>6.1590091567837797E-2</v>
       </c>
       <c r="D19">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$Q$2:$Q$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$Q$2:$Q$1001)</f>
         <v>0.25757747543461812</v>
       </c>
       <c r="E19">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$Q$2:$Q$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$Q$2:$Q$1001)</f>
         <v>7.7756852756210193E-2</v>
       </c>
     </row>
@@ -31965,19 +31966,19 @@
         <v>85</v>
       </c>
       <c r="B20">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$R$2:$R$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$R$2:$R$1001)</f>
         <v>6.2037254659409402E-2</v>
       </c>
       <c r="C20">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$R$2:$R$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$R$2:$R$1001)</f>
         <v>7.2381489779792488E-2</v>
       </c>
       <c r="D20">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$R$2:$R$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$R$2:$R$1001)</f>
         <v>0.17968734537357722</v>
       </c>
       <c r="E20">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$R$2:$R$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$R$2:$R$1001)</f>
         <v>9.3550773096804971E-2</v>
       </c>
     </row>
@@ -31986,19 +31987,19 @@
         <v>90</v>
       </c>
       <c r="B21">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$S$2:$S$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$S$2:$S$1001)</f>
         <v>8.7544327653023044E-2</v>
       </c>
       <c r="C21">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$S$2:$S$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$S$2:$S$1001)</f>
         <v>0.11010273546227865</v>
       </c>
       <c r="D21">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$S$2:$S$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$S$2:$S$1001)</f>
         <v>0.14326670913627415</v>
       </c>
       <c r="E21">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$S$2:$S$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$S$2:$S$1001)</f>
         <v>0.12028777565835862</v>
       </c>
     </row>
@@ -32007,19 +32008,19 @@
         <v>95</v>
       </c>
       <c r="B22">
-        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$T$2:$T$101)</f>
+        <f>AVERAGE('[3]ari-eval-tracesec-cwa'!$T$2:$T$1001)</f>
         <v>4.106172501823574E-2</v>
       </c>
       <c r="C22">
-        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$T$2:$T$101)</f>
+        <f>_xlfn.STDEV.P('[3]ari-eval-tracesec-cwa'!$T$2:$T$1001)</f>
         <v>0.12114631056966503</v>
       </c>
       <c r="D22">
-        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$T$2:$T$101)</f>
+        <f>AVERAGE('[4]ari-eval-sonarcube-cwa'!$T$2:$T$1001)</f>
         <v>8.5746489788476113E-2</v>
       </c>
       <c r="E22">
-        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$T$2:$T$101)</f>
+        <f>_xlfn.STDEV.P('[4]ari-eval-sonarcube-cwa'!$T$2:$T$1001)</f>
         <v>0.14030917046780314</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed typo and added merged result plot
</commit_message>
<xml_diff>
--- a/ARIevaluation/PrioTopK/output/topkanalysis.xlsx
+++ b/ARIevaluation/PrioTopK/output/topkanalysis.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\TraceSec\tracesec-prioritization\ARIevaluation\PrioTopK\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECDD151-2BA7-48A5-BCB3-0020E9232616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FAD2E5-AFB1-45BE-9EA3-1891B6B37FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{9F6FB41D-B757-4B1F-BB02-0258B271A8C4}"/>
+    <workbookView xWindow="-18120" yWindow="-120" windowWidth="18240" windowHeight="28320" xr2:uid="{9F6FB41D-B757-4B1F-BB02-0258B271A8C4}"/>
   </bookViews>
   <sheets>
     <sheet name="itrust" sheetId="3" r:id="rId1"/>
     <sheet name="cwa" sheetId="2" r:id="rId2"/>
+    <sheet name="plot" sheetId="5" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,9 +47,6 @@
     <t>TraceSec</t>
   </si>
   <si>
-    <t>SonarCube</t>
-  </si>
-  <si>
     <t>ARI</t>
   </si>
   <si>
@@ -56,6 +54,9 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>SonarQube</t>
   </si>
 </sst>
 </file>
@@ -118,8 +119,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF250599"/>
       <color rgb="FF12247C"/>
-      <color rgb="FF250599"/>
     </mruColors>
   </colors>
   <extLst>
@@ -547,7 +548,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SonarCube</c:v>
+                  <c:v>SonarQube</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1245,8 +1246,8 @@
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -1323,7 +1324,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SonarCube</c:v>
+                  <c:v>SonarQube</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1717,25 +1718,8 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Adjusted Rand Index vs.</a:t>
+                  <a:t>Adjusted Rand Index</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> Manual</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1200">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2286,7 +2270,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SonarCube</c:v>
+                  <c:v>SonarQube</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2985,8 +2969,8 @@
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -3063,7 +3047,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SonarCube</c:v>
+                  <c:v>SonarQube</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3457,7 +3441,7 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Adjusted Rand Index vs. Manual</a:t>
+                  <a:t>Adjusted Rand Index</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3592,6 +3576,1180 @@
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TraceSec CWA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="12247C"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>cwa!$C$3:$C$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>0.12867261615639375</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.11973861986098269</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.10086693732254118</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.9988658329439726E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.3306690738754696E-16</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1189331631568264E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.9077050110947996E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.6841959535943776E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.0944394382645218E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.4343734632924894E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.0928298587505169E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1.9314631224775343E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.0295602551673127E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.6170736318086663E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.6328677795507166E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>5.2351133696630102E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>6.1590091567837797E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>7.2381489779792488E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>0.11010273546227865</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.12114631056966503</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>cwa!$C$3:$C$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>0.12867261615639375</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.11973861986098269</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.10086693732254118</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.9988658329439726E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.3306690738754696E-16</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.1189331631568264E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.9077050110947996E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.6841959535943776E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.0944394382645218E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.4343734632924894E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.0928298587505169E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1.9314631224775343E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.0295602551673127E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.6170736318086663E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.6328677795507166E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>5.2351133696630102E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>6.1590091567837797E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>7.2381489779792488E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>0.11010273546227865</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.12114631056966503</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>cwa!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cwa!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.5142348057643868E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12252122538353798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15589590486142138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23060557149689029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33369542178889267</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19840752688171931</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-80AB-4356-A217-047FC21019A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SonarQube CWA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>cwa!$E$3:$E$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>8.3266726846886741E-17</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.2588895335479784E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.2468542601595951E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.7610192502172622E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.1144762478002467E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.5682156262949339E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.4172942829946195E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.9734826227852972E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.1591995460654589E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.1631863482203086E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1706922282435046E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.7848959709662158E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.7305796781177521E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>4.7453942117821259E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>6.3328218307908413E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>7.924567131691275E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>7.7756852756210193E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>9.3550773096804971E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>0.12028777565835862</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.14030917046780314</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>cwa!$E$3:$E$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>8.3266726846886741E-17</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.2588895335479784E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.2468542601595951E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.7610192502172622E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.1144762478002467E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.5682156262949339E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.4172942829946195E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.9734826227852972E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.1591995460654589E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.1631863482203086E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.1706922282435046E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.7848959709662158E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.7305796781177521E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>4.7453942117821259E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>6.3328218307908413E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>7.924567131691275E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>7.7756852756210193E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>9.3550773096804971E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>0.12028777565835862</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.14030917046780314</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>cwa!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cwa!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-5.6038533834586284E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.6038533834586284E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.6825894412103729E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5741072851904736E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8826656775469842E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5545574855252126E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-80AB-4356-A217-047FC21019A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>TraceSec iTrust</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>itrust!$C$3:$C$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>7.3674395964506381E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3777125409855005E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.8975420584322224E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.9972616848872256E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.7663859249626072E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.8509270337876942E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.1102230246251565E-16</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.9635753171232997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.8591659000537889E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.847636915277036E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.6731020840490687E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.344027074132002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.8450788039703865E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.9632516614715209E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.3001863515958159E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>4.8977742958372074E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.8901602817265429E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>4.5326919415885396E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>8.3436850647333E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.15738520347472759</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>itrust!$C$3:$C$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>7.3674395964506381E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3777125409855005E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.8975420584322224E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.9972616848872256E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.7663859249626072E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.8509270337876942E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.1102230246251565E-16</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.9635753171232997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.8591659000537889E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.847636915277036E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.6731020840490687E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.344027074132002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.8450788039703865E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.9632516614715209E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.3001863515958159E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>4.8977742958372074E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.8901602817265429E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>4.5326919415885396E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>8.3436850647333E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.15738520347472759</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>itrust!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>itrust!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.14547253834735224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14932097594232027</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15454460569465642</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19704510339909614</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26811244211980328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35668970103867587</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-80AB-4356-A217-047FC21019A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>SonarQube iTrust</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>itrust!$E$3:$E$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>6.9293960224273865E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5900099257370651E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.2878585564539262E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.560327922685379E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.5701749244413313E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.6000658900812924E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.4497534575950848E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.01231640414617E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.4886804588892303E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.032717313399871E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.7046891643746074E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.1954762352262493E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.9146679704781504E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.3613275756784357E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.0506241159845057E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.4363434621418325E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>4.9735134601080144E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>7.0147064208879853E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>7.2889251620383677E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>5.2915551091664355E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>itrust!$E$3:$E$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="20"/>
+                  <c:pt idx="0">
+                    <c:v>6.9293960224273865E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5900099257370651E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.2878585564539262E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.560327922685379E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.5701749244413313E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.6000658900812924E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.4497534575950848E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.01231640414617E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.4886804588892303E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.032717313399871E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.7046891643746074E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.1954762352262493E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.9146679704781504E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.3613275756784357E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.0506241159845057E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.4363434621418325E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>4.9735134601080144E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>7.0147064208879853E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>7.2889251620383677E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>5.2915551091664355E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>itrust!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>itrust!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-1.4411182582880201E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.6561562382419442E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8420203780781119E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13782646482053665</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2127353739691179</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30411210946571132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-80AB-4356-A217-047FC21019A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="528927120"/>
+        <c:axId val="528934320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="528927120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528934320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="528934320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.45"/>
+          <c:min val="-0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Adjusted Rand Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="528927120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -5767,6 +6925,17 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{724DA951-D6DA-46D0-823F-02961CBDE321}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5922,6 +7091,39 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9300882" cy="6011155"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCB14477-5490-56EB-5F10-A96AAA65FA6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -31092,44 +32294,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39CD883-F74C-47E5-932D-444A56709C19}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+      <c r="D2" t="s">
+        <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -31150,7 +32352,7 @@
         <v>6.9293960224273865E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -31171,7 +32373,7 @@
         <v>7.5900099257370651E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -31192,7 +32394,7 @@
         <v>9.2878585564539262E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -31213,7 +32415,7 @@
         <v>8.560327922685379E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -31234,7 +32436,7 @@
         <v>6.5701749244413313E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -31255,7 +32457,7 @@
         <v>4.6000658900812924E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -31276,7 +32478,7 @@
         <v>4.4497534575950848E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>35</v>
       </c>
@@ -31297,7 +32499,7 @@
         <v>5.01231640414617E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>40</v>
       </c>
@@ -31318,7 +32520,7 @@
         <v>3.4886804588892303E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>45</v>
       </c>
@@ -31339,7 +32541,7 @@
         <v>3.032717313399871E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
@@ -31360,7 +32562,7 @@
         <v>2.7046891643746074E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>55</v>
       </c>
@@ -31381,7 +32583,7 @@
         <v>2.1954762352262493E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>60</v>
       </c>
@@ -31402,7 +32604,7 @@
         <v>1.9146679704781504E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>65</v>
       </c>
@@ -31423,7 +32625,7 @@
         <v>2.3613275756784357E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70</v>
       </c>
@@ -31444,7 +32646,7 @@
         <v>3.0506241159845057E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>75</v>
       </c>
@@ -31465,7 +32667,7 @@
         <v>3.4363434621418325E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>80</v>
       </c>
@@ -31486,7 +32688,7 @@
         <v>4.9735134601080144E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>85</v>
       </c>
@@ -31507,7 +32709,7 @@
         <v>7.0147064208879853E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90</v>
       </c>
@@ -31528,7 +32730,7 @@
         <v>7.2889251620383677E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>95</v>
       </c>
@@ -31567,44 +32769,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9864635-2355-44AC-9B5A-8CDFEFA8D606}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+      <c r="D2" t="s">
+        <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -31625,7 +32827,7 @@
         <v>8.3266726846886741E-17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -31646,7 +32848,7 @@
         <v>4.2588895335479784E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -31667,7 +32869,7 @@
         <v>7.2468542601595951E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -31688,7 +32890,7 @@
         <v>6.7610192502172622E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -31709,7 +32911,7 @@
         <v>5.1144762478002467E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -31730,7 +32932,7 @@
         <v>5.5682156262949339E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -31751,7 +32953,7 @@
         <v>4.4172942829946195E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>35</v>
       </c>
@@ -31772,7 +32974,7 @@
         <v>2.9734826227852972E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>40</v>
       </c>
@@ -31793,7 +32995,7 @@
         <v>3.1591995460654589E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>45</v>
       </c>
@@ -31814,7 +33016,7 @@
         <v>3.1631863482203086E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
@@ -31835,7 +33037,7 @@
         <v>3.1706922282435046E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>55</v>
       </c>
@@ -31856,7 +33058,7 @@
         <v>2.7848959709662158E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>60</v>
       </c>
@@ -31877,7 +33079,7 @@
         <v>3.7305796781177521E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>65</v>
       </c>
@@ -31898,7 +33100,7 @@
         <v>4.7453942117821259E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70</v>
       </c>
@@ -31919,7 +33121,7 @@
         <v>6.3328218307908413E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>75</v>
       </c>
@@ -31940,7 +33142,7 @@
         <v>7.924567131691275E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>80</v>
       </c>
@@ -31961,7 +33163,7 @@
         <v>7.7756852756210193E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>85</v>
       </c>
@@ -31982,7 +33184,7 @@
         <v>9.3550773096804971E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90</v>
       </c>
@@ -32003,7 +33205,7 @@
         <v>0.12028777565835862</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>95</v>
       </c>

</xml_diff>